<commit_message>
Adjusted data input and crude hyper parameter tuning for svm
</commit_message>
<xml_diff>
--- a/src/results.xlsx
+++ b/src/results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Working\UIC\Fall2018\CS583\Project2\CS583FinalProject\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{560ABD56-C174-4555-A36C-95E48CDFD988}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5463854-DD20-4E32-B277-52B9D0E6A5F3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19020" windowHeight="4365" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19020" windowHeight="4365" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test" sheetId="1" r:id="rId1"/>
+    <sheet name="test_results" sheetId="1" r:id="rId1"/>
     <sheet name="Charts" sheetId="2" r:id="rId2"/>
+    <sheet name="train_results" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
   <si>
     <t>nn</t>
   </si>
@@ -88,13 +96,25 @@
   <si>
     <t>scenario</t>
   </si>
+  <si>
+    <t>NN_TFIDF</t>
+  </si>
+  <si>
+    <t>NN_Custom</t>
+  </si>
+  <si>
+    <t>RandomForest_TFIDF</t>
+  </si>
+  <si>
+    <t>RandomForest_Custom</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -589,7 +609,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -691,11 +711,6 @@
               <a:rPr lang="en-US"/>
               <a:t>Accuracy</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> by Scenario</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -750,7 +765,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>test!$D$2:$D$17</c:f>
+              <c:f>test_results!$D$2:$D$17</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -806,7 +821,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>test!$E$2:$E$17</c:f>
+              <c:f>test_results!$E$2:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -935,6 +950,7 @@
         <c:axId val="505689936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1074,13 +1090,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>f1_positive</a:t>
+              <a:t>f_positive</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> by scenario </a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1135,7 +1146,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>test!$D$2:$D$17</c:f>
+              <c:f>test_results!$D$2:$D$17</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -1191,7 +1202,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>test!$F$2:$F$17</c:f>
+              <c:f>test_results!$F$2:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1459,7 +1470,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>f1_neutral by scenario</a:t>
+              <a:t>f_neutral</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1515,7 +1526,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>test!$D$2:$D$17</c:f>
+              <c:f>test_results!$D$2:$D$17</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -1571,7 +1582,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>test!$I$2:$I$17</c:f>
+              <c:f>test_results!$I$2:$I$17</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1839,7 +1850,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>f1_negative by scenario</a:t>
+              <a:t>f_negative</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1895,7 +1906,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>test!$D$2:$D$17</c:f>
+              <c:f>test_results!$D$2:$D$17</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -1951,7 +1962,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>test!$L$2:$L$17</c:f>
+              <c:f>test_results!$L$2:$L$17</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2129,6 +2140,321 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="398910776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Custom V TF-IDF</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> in Train</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="B33C2F"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>train_results!$A$1:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>NN_Custom</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NN_TFIDF</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RandomForest_Custom</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RandomForest_TFIDF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>train_results!$B$1:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91700000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-59B7-4340-872E-70F78CEE1A05}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="498181480"/>
+        <c:axId val="498182136"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="498181480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="498182136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="498182136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="498181480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2344,6 +2670,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3854,6 +4220,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4513,6 +5382,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9964CC8F-EB86-4FCF-9241-893B87724B7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4809,11 +5719,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4889,7 +5799,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="str">
-        <f>A2&amp;"_"&amp;B2&amp;"_"&amp;C2</f>
+        <f t="shared" ref="D2:D17" si="0">A2&amp;"_"&amp;B2&amp;"_"&amp;C2</f>
         <v>data-1_train.csv_rf_tfidf</v>
       </c>
       <c r="E2" s="3">
@@ -4934,7 +5844,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f>A3&amp;"_"&amp;B3&amp;"_"&amp;C3</f>
+        <f t="shared" si="0"/>
         <v>data-1_train.csv_nn_tfidf</v>
       </c>
       <c r="E3" s="3">
@@ -4979,7 +5889,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="str">
-        <f>A4&amp;"_"&amp;B4&amp;"_"&amp;C4</f>
+        <f t="shared" si="0"/>
         <v>data-1_train.csv_nn_cust</v>
       </c>
       <c r="E4" s="3">
@@ -5024,7 +5934,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="str">
-        <f>A5&amp;"_"&amp;B5&amp;"_"&amp;C5</f>
+        <f t="shared" si="0"/>
         <v>data-1_train.csv_rf_cust</v>
       </c>
       <c r="E5" s="3">
@@ -5069,7 +5979,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="str">
-        <f>A6&amp;"_"&amp;B6&amp;"_"&amp;C6</f>
+        <f t="shared" si="0"/>
         <v>data-1_train.csv_dt_tfidf</v>
       </c>
       <c r="E6" s="3">
@@ -5114,7 +6024,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="1" t="str">
-        <f>A7&amp;"_"&amp;B7&amp;"_"&amp;C7</f>
+        <f t="shared" si="0"/>
         <v>data-1_train.csv_nb_cust</v>
       </c>
       <c r="E7" s="3">
@@ -5159,7 +6069,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="str">
-        <f>A8&amp;"_"&amp;B8&amp;"_"&amp;C8</f>
+        <f t="shared" si="0"/>
         <v>data-1_train.csv_nb_tfidf</v>
       </c>
       <c r="E8" s="3">
@@ -5204,7 +6114,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="str">
-        <f>A9&amp;"_"&amp;B9&amp;"_"&amp;C9</f>
+        <f t="shared" si="0"/>
         <v>data-1_train.csv_dt_cust</v>
       </c>
       <c r="E9" s="3">
@@ -5249,7 +6159,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="1" t="str">
-        <f>A10&amp;"_"&amp;B10&amp;"_"&amp;C10</f>
+        <f t="shared" si="0"/>
         <v>data-2_train.csv_nn_cust</v>
       </c>
       <c r="E10" s="3">
@@ -5294,7 +6204,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="1" t="str">
-        <f>A11&amp;"_"&amp;B11&amp;"_"&amp;C11</f>
+        <f t="shared" si="0"/>
         <v>data-2_train.csv_rf_cust</v>
       </c>
       <c r="E11" s="3">
@@ -5339,7 +6249,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="str">
-        <f>A12&amp;"_"&amp;B12&amp;"_"&amp;C12</f>
+        <f t="shared" si="0"/>
         <v>data-2_train.csv_rf_tfidf</v>
       </c>
       <c r="E12" s="3">
@@ -5384,7 +6294,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="str">
-        <f>A13&amp;"_"&amp;B13&amp;"_"&amp;C13</f>
+        <f t="shared" si="0"/>
         <v>data-2_train.csv_nn_tfidf</v>
       </c>
       <c r="E13" s="3">
@@ -5429,7 +6339,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="str">
-        <f>A14&amp;"_"&amp;B14&amp;"_"&amp;C14</f>
+        <f t="shared" si="0"/>
         <v>data-2_train.csv_dt_tfidf</v>
       </c>
       <c r="E14" s="3">
@@ -5474,7 +6384,7 @@
         <v>3</v>
       </c>
       <c r="D15" s="1" t="str">
-        <f>A15&amp;"_"&amp;B15&amp;"_"&amp;C15</f>
+        <f t="shared" si="0"/>
         <v>data-2_train.csv_dt_cust</v>
       </c>
       <c r="E15" s="3">
@@ -5519,7 +6429,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="str">
-        <f>A16&amp;"_"&amp;B16&amp;"_"&amp;C16</f>
+        <f t="shared" si="0"/>
         <v>data-2_train.csv_nb_cust</v>
       </c>
       <c r="E16" s="3">
@@ -5564,7 +6474,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="1" t="str">
-        <f>A17&amp;"_"&amp;B17&amp;"_"&amp;C17</f>
+        <f t="shared" si="0"/>
         <v>data-2_train.csv_nb_tfidf</v>
       </c>
       <c r="E17" s="3">
@@ -5608,11 +6518,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5620,4 +6530,52 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFB9D0E-A095-49B4-98EB-5E3266418114}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>0.90100000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>0.99199999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>